<commit_message>
fixed problem with NAs in LG bias calculation
</commit_message>
<xml_diff>
--- a/LG_ages.xlsx
+++ b/LG_ages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK-Online-Replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2A2132-1FA9-FF41-9F4E-930AD4AF1457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7332939-E221-B344-907F-084DD930436F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="500" windowWidth="13240" windowHeight="13660" xr2:uid="{37D332D1-B1CD-6647-A08F-6000C2E6D55A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -310,6 +310,27 @@
   </si>
   <si>
     <t>blg049</t>
+  </si>
+  <si>
+    <t>blg050</t>
+  </si>
+  <si>
+    <t>blg051</t>
+  </si>
+  <si>
+    <t>blg052</t>
+  </si>
+  <si>
+    <t>blg053</t>
+  </si>
+  <si>
+    <t>blg054</t>
+  </si>
+  <si>
+    <t>blg057</t>
+  </si>
+  <si>
+    <t>blg058</t>
   </si>
 </sst>
 </file>
@@ -714,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8720D5E-9B7F-1345-B316-31B8EB44D7A1}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1526,63 +1547,85 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
-        <v>71</v>
+      <c r="A74" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="B74" s="3">
-        <v>23</v>
-      </c>
-      <c r="C74" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>72</v>
+      <c r="A75" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="B75" s="3">
-        <v>21</v>
-      </c>
-      <c r="C75" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>73</v>
+        <v>11</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="B76" s="3">
-        <v>19</v>
-      </c>
-      <c r="C76" t="s">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
-        <v>74</v>
+      <c r="A77" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="B77" s="3">
-        <v>20</v>
-      </c>
-      <c r="C77" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
-        <v>75</v>
+      <c r="A78" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="B78" s="3">
-        <v>22</v>
-      </c>
-      <c r="C78" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B79" s="3">
+        <v>11</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B80" s="3">
+        <v>9</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C78">
-    <sortCondition ref="A1:A78"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C73">
+    <sortCondition ref="A1:A73"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1591,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6608F609-BBE6-C74C-A38F-ED8DF40111DA}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="A8" sqref="A8:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1676,6 +1719,61 @@
         <v>30</v>
       </c>
     </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="3">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="3">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="3">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="3">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="3">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>